<commit_message>
adding Scorecard documentation pdf - update as needed
</commit_message>
<xml_diff>
--- a/between_states/between_states_relative_data/combined_category_scores_between_2022_excel.xlsx
+++ b/between_states/between_states_relative_data/combined_category_scores_between_2022_excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>Table 1</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>DE</t>
-  </si>
-  <si>
-    <t>District of Columbia</t>
-  </si>
-  <si>
-    <t>DC</t>
   </si>
   <si>
     <t>Florida</t>
@@ -767,7 +761,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="ffffffff"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="20"/>
+          <bgColor indexed="21"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ffffffff"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="20"/>
+          <bgColor indexed="23"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="20"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="ffffffff"/>
@@ -1890,7 +1917,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:H54"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="E3" xSplit="4" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2176,7 +2203,7 @@
     </row>
     <row r="12" ht="24.7" customHeight="1">
       <c r="A12" s="16">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s" s="17">
         <v>27</v>
@@ -2188,21 +2215,21 @@
         <v>2022</v>
       </c>
       <c r="E12" s="12">
-        <v>40.33</v>
+        <v>53.37</v>
       </c>
       <c r="F12" s="20">
-        <v>47.84</v>
+        <v>49.09</v>
       </c>
       <c r="G12" s="21">
-        <v>43.1</v>
+        <v>48.23</v>
       </c>
       <c r="H12" s="22">
-        <v>43.75</v>
+        <v>50.24</v>
       </c>
     </row>
     <row r="13" ht="24.7" customHeight="1">
       <c r="A13" s="16">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s" s="17">
         <v>29</v>
@@ -2214,21 +2241,21 @@
         <v>2022</v>
       </c>
       <c r="E13" s="12">
-        <v>53.37</v>
+        <v>61.16</v>
       </c>
       <c r="F13" s="20">
-        <v>49.09</v>
+        <v>48.31</v>
       </c>
       <c r="G13" s="21">
-        <v>48.23</v>
+        <v>49.28</v>
       </c>
       <c r="H13" s="22">
-        <v>50.24</v>
+        <v>52.93</v>
       </c>
     </row>
     <row r="14" ht="24.7" customHeight="1">
       <c r="A14" s="16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s" s="17">
         <v>31</v>
@@ -2240,21 +2267,21 @@
         <v>2022</v>
       </c>
       <c r="E14" s="12">
-        <v>61.16</v>
+        <v>55.31</v>
       </c>
       <c r="F14" s="20">
-        <v>48.31</v>
+        <v>54.54</v>
       </c>
       <c r="G14" s="21">
-        <v>49.28</v>
+        <v>62.39</v>
       </c>
       <c r="H14" s="22">
-        <v>52.93</v>
+        <v>57.41</v>
       </c>
     </row>
     <row r="15" ht="24.7" customHeight="1">
       <c r="A15" s="16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s" s="17">
         <v>33</v>
@@ -2266,21 +2293,21 @@
         <v>2022</v>
       </c>
       <c r="E15" s="12">
-        <v>55.31</v>
+        <v>42.62</v>
       </c>
       <c r="F15" s="20">
-        <v>54.54</v>
+        <v>52.37</v>
       </c>
       <c r="G15" s="21">
-        <v>62.39</v>
+        <v>56.68</v>
       </c>
       <c r="H15" s="22">
-        <v>57.41</v>
+        <v>50.55</v>
       </c>
     </row>
     <row r="16" ht="24.7" customHeight="1">
       <c r="A16" s="16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s" s="17">
         <v>35</v>
@@ -2292,21 +2319,21 @@
         <v>2022</v>
       </c>
       <c r="E16" s="12">
-        <v>42.62</v>
+        <v>47.39</v>
       </c>
       <c r="F16" s="20">
-        <v>52.37</v>
+        <v>49.95</v>
       </c>
       <c r="G16" s="21">
-        <v>56.68</v>
+        <v>47.27</v>
       </c>
       <c r="H16" s="22">
-        <v>50.55</v>
+        <v>48.21</v>
       </c>
     </row>
     <row r="17" ht="24.7" customHeight="1">
       <c r="A17" s="16">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s" s="17">
         <v>37</v>
@@ -2318,21 +2345,21 @@
         <v>2022</v>
       </c>
       <c r="E17" s="12">
-        <v>47.39</v>
+        <v>48.92</v>
       </c>
       <c r="F17" s="20">
-        <v>49.95</v>
+        <v>49.84</v>
       </c>
       <c r="G17" s="21">
-        <v>47.27</v>
+        <v>51.16</v>
       </c>
       <c r="H17" s="22">
-        <v>48.21</v>
+        <v>49.97</v>
       </c>
     </row>
     <row r="18" ht="24.7" customHeight="1">
       <c r="A18" s="16">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s" s="17">
         <v>39</v>
@@ -2344,21 +2371,21 @@
         <v>2022</v>
       </c>
       <c r="E18" s="12">
-        <v>48.92</v>
+        <v>39.98</v>
       </c>
       <c r="F18" s="20">
-        <v>49.84</v>
+        <v>48.43</v>
       </c>
       <c r="G18" s="21">
-        <v>51.16</v>
+        <v>56.07</v>
       </c>
       <c r="H18" s="22">
-        <v>49.97</v>
+        <v>48.17</v>
       </c>
     </row>
     <row r="19" ht="24.7" customHeight="1">
       <c r="A19" s="16">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s" s="17">
         <v>41</v>
@@ -2370,21 +2397,21 @@
         <v>2022</v>
       </c>
       <c r="E19" s="12">
-        <v>39.98</v>
+        <v>42</v>
       </c>
       <c r="F19" s="20">
-        <v>48.43</v>
+        <v>47.43</v>
       </c>
       <c r="G19" s="21">
-        <v>56.07</v>
+        <v>58.11</v>
       </c>
       <c r="H19" s="22">
-        <v>48.17</v>
+        <v>49.18</v>
       </c>
     </row>
     <row r="20" ht="24.7" customHeight="1">
       <c r="A20" s="16">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s" s="17">
         <v>43</v>
@@ -2396,21 +2423,21 @@
         <v>2022</v>
       </c>
       <c r="E20" s="12">
-        <v>42</v>
+        <v>51.75</v>
       </c>
       <c r="F20" s="20">
-        <v>47.43</v>
+        <v>49.85</v>
       </c>
       <c r="G20" s="21">
-        <v>58.11</v>
+        <v>39.3</v>
       </c>
       <c r="H20" s="22">
-        <v>49.18</v>
+        <v>46.98</v>
       </c>
     </row>
     <row r="21" ht="24.7" customHeight="1">
       <c r="A21" s="16">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s" s="17">
         <v>45</v>
@@ -2422,21 +2449,21 @@
         <v>2022</v>
       </c>
       <c r="E21" s="12">
-        <v>51.75</v>
+        <v>55.66</v>
       </c>
       <c r="F21" s="20">
-        <v>49.85</v>
+        <v>46.73</v>
       </c>
       <c r="G21" s="21">
-        <v>39.3</v>
+        <v>39.25</v>
       </c>
       <c r="H21" s="22">
-        <v>46.98</v>
+        <v>47.23</v>
       </c>
     </row>
     <row r="22" ht="24.7" customHeight="1">
       <c r="A22" s="16">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s" s="17">
         <v>47</v>
@@ -2448,21 +2475,21 @@
         <v>2022</v>
       </c>
       <c r="E22" s="12">
-        <v>55.66</v>
+        <v>44.57</v>
       </c>
       <c r="F22" s="20">
-        <v>46.73</v>
+        <v>50.46</v>
       </c>
       <c r="G22" s="21">
-        <v>39.25</v>
+        <v>44.97</v>
       </c>
       <c r="H22" s="22">
-        <v>47.23</v>
+        <v>46.68</v>
       </c>
     </row>
     <row r="23" ht="24.7" customHeight="1">
       <c r="A23" s="16">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s" s="17">
         <v>49</v>
@@ -2474,21 +2501,21 @@
         <v>2022</v>
       </c>
       <c r="E23" s="12">
-        <v>44.57</v>
+        <v>50.32</v>
       </c>
       <c r="F23" s="20">
-        <v>50.46</v>
+        <v>56.64</v>
       </c>
       <c r="G23" s="21">
-        <v>44.97</v>
+        <v>58.32</v>
       </c>
       <c r="H23" s="22">
-        <v>46.68</v>
+        <v>55.09</v>
       </c>
     </row>
     <row r="24" ht="24.7" customHeight="1">
       <c r="A24" s="16">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s" s="17">
         <v>51</v>
@@ -2500,21 +2527,21 @@
         <v>2022</v>
       </c>
       <c r="E24" s="12">
-        <v>50.32</v>
+        <v>44.82</v>
       </c>
       <c r="F24" s="20">
-        <v>56.64</v>
+        <v>51.03</v>
       </c>
       <c r="G24" s="21">
-        <v>58.32</v>
+        <v>48.04</v>
       </c>
       <c r="H24" s="22">
-        <v>55.09</v>
+        <v>47.96</v>
       </c>
     </row>
     <row r="25" ht="24.7" customHeight="1">
       <c r="A25" s="16">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s" s="17">
         <v>53</v>
@@ -2526,21 +2553,21 @@
         <v>2022</v>
       </c>
       <c r="E25" s="12">
-        <v>44.82</v>
+        <v>50.92</v>
       </c>
       <c r="F25" s="20">
-        <v>51.03</v>
+        <v>54.49</v>
       </c>
       <c r="G25" s="21">
-        <v>48.04</v>
+        <v>41.06</v>
       </c>
       <c r="H25" s="22">
-        <v>47.96</v>
+        <v>48.82</v>
       </c>
     </row>
     <row r="26" ht="24.7" customHeight="1">
       <c r="A26" s="16">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s" s="17">
         <v>55</v>
@@ -2552,21 +2579,21 @@
         <v>2022</v>
       </c>
       <c r="E26" s="12">
-        <v>50.92</v>
+        <v>40.91</v>
       </c>
       <c r="F26" s="20">
-        <v>54.49</v>
+        <v>50.71</v>
       </c>
       <c r="G26" s="21">
-        <v>41.06</v>
+        <v>55.84</v>
       </c>
       <c r="H26" s="22">
-        <v>48.82</v>
+        <v>49.15</v>
       </c>
     </row>
     <row r="27" ht="24.7" customHeight="1">
       <c r="A27" s="16">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s" s="17">
         <v>57</v>
@@ -2578,21 +2605,21 @@
         <v>2022</v>
       </c>
       <c r="E27" s="12">
-        <v>40.91</v>
+        <v>54.73</v>
       </c>
       <c r="F27" s="20">
-        <v>50.71</v>
+        <v>41.07</v>
       </c>
       <c r="G27" s="21">
-        <v>55.84</v>
+        <v>37.78</v>
       </c>
       <c r="H27" s="22">
-        <v>49.15</v>
+        <v>44.52</v>
       </c>
     </row>
     <row r="28" ht="24.7" customHeight="1">
       <c r="A28" s="16">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s" s="17">
         <v>59</v>
@@ -2604,21 +2631,21 @@
         <v>2022</v>
       </c>
       <c r="E28" s="12">
-        <v>54.73</v>
+        <v>45.99</v>
       </c>
       <c r="F28" s="20">
-        <v>41.07</v>
+        <v>44.34</v>
       </c>
       <c r="G28" s="21">
-        <v>37.78</v>
+        <v>47.19</v>
       </c>
       <c r="H28" s="22">
-        <v>44.52</v>
+        <v>45.84</v>
       </c>
     </row>
     <row r="29" ht="24.7" customHeight="1">
       <c r="A29" s="16">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s" s="17">
         <v>61</v>
@@ -2630,21 +2657,21 @@
         <v>2022</v>
       </c>
       <c r="E29" s="12">
-        <v>45.99</v>
+        <v>48.12</v>
       </c>
       <c r="F29" s="20">
-        <v>44.34</v>
+        <v>50.24</v>
       </c>
       <c r="G29" s="21">
-        <v>47.19</v>
+        <v>55.98</v>
       </c>
       <c r="H29" s="22">
-        <v>45.84</v>
+        <v>51.44</v>
       </c>
     </row>
     <row r="30" ht="24.7" customHeight="1">
       <c r="A30" s="16">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s" s="17">
         <v>63</v>
@@ -2656,21 +2683,21 @@
         <v>2022</v>
       </c>
       <c r="E30" s="12">
-        <v>48.12</v>
+        <v>49.77</v>
       </c>
       <c r="F30" s="20">
-        <v>50.24</v>
+        <v>48.9</v>
       </c>
       <c r="G30" s="21">
-        <v>55.98</v>
+        <v>64.52</v>
       </c>
       <c r="H30" s="22">
-        <v>51.44</v>
+        <v>54.41</v>
       </c>
     </row>
     <row r="31" ht="24.7" customHeight="1">
       <c r="A31" s="16">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s" s="17">
         <v>65</v>
@@ -2682,21 +2709,21 @@
         <v>2022</v>
       </c>
       <c r="E31" s="12">
-        <v>49.77</v>
+        <v>61.91</v>
       </c>
       <c r="F31" s="20">
-        <v>48.9</v>
+        <v>56.53</v>
       </c>
       <c r="G31" s="21">
-        <v>64.52</v>
+        <v>53.26</v>
       </c>
       <c r="H31" s="22">
-        <v>54.41</v>
+        <v>57.23</v>
       </c>
     </row>
     <row r="32" ht="24.7" customHeight="1">
       <c r="A32" s="16">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s" s="17">
         <v>67</v>
@@ -2708,21 +2735,21 @@
         <v>2022</v>
       </c>
       <c r="E32" s="12">
-        <v>61.91</v>
+        <v>40.27</v>
       </c>
       <c r="F32" s="20">
-        <v>56.53</v>
+        <v>52.3</v>
       </c>
       <c r="G32" s="21">
-        <v>53.26</v>
+        <v>57.43</v>
       </c>
       <c r="H32" s="22">
-        <v>57.23</v>
+        <v>50.01</v>
       </c>
     </row>
     <row r="33" ht="24.7" customHeight="1">
       <c r="A33" s="16">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s" s="17">
         <v>69</v>
@@ -2734,21 +2761,21 @@
         <v>2022</v>
       </c>
       <c r="E33" s="12">
-        <v>40.27</v>
+        <v>56.84</v>
       </c>
       <c r="F33" s="20">
-        <v>52.3</v>
+        <v>54.12</v>
       </c>
       <c r="G33" s="21">
-        <v>57.43</v>
+        <v>52.58</v>
       </c>
       <c r="H33" s="22">
-        <v>50.01</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="34" ht="24.7" customHeight="1">
       <c r="A34" s="16">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s" s="17">
         <v>71</v>
@@ -2760,21 +2787,21 @@
         <v>2022</v>
       </c>
       <c r="E34" s="12">
-        <v>56.84</v>
+        <v>54.31</v>
       </c>
       <c r="F34" s="20">
-        <v>54.12</v>
+        <v>49.52</v>
       </c>
       <c r="G34" s="21">
-        <v>52.58</v>
+        <v>39.24</v>
       </c>
       <c r="H34" s="22">
-        <v>54.5</v>
+        <v>47.69</v>
       </c>
     </row>
     <row r="35" ht="24.7" customHeight="1">
       <c r="A35" s="16">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s" s="17">
         <v>73</v>
@@ -2786,21 +2813,21 @@
         <v>2022</v>
       </c>
       <c r="E35" s="12">
-        <v>54.31</v>
+        <v>47.54</v>
       </c>
       <c r="F35" s="20">
-        <v>49.52</v>
+        <v>48.98</v>
       </c>
       <c r="G35" s="21">
-        <v>39.24</v>
+        <v>41.34</v>
       </c>
       <c r="H35" s="22">
-        <v>47.69</v>
+        <v>45.94</v>
       </c>
     </row>
     <row r="36" ht="24.7" customHeight="1">
       <c r="A36" s="16">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s" s="17">
         <v>75</v>
@@ -2812,21 +2839,21 @@
         <v>2022</v>
       </c>
       <c r="E36" s="12">
-        <v>47.54</v>
+        <v>56.46</v>
       </c>
       <c r="F36" s="20">
-        <v>48.98</v>
+        <v>48.92</v>
       </c>
       <c r="G36" s="21">
-        <v>41.34</v>
+        <v>45.92</v>
       </c>
       <c r="H36" s="22">
-        <v>45.94</v>
+        <v>50.45</v>
       </c>
     </row>
     <row r="37" ht="24.7" customHeight="1">
       <c r="A37" s="16">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s" s="17">
         <v>77</v>
@@ -2838,21 +2865,21 @@
         <v>2022</v>
       </c>
       <c r="E37" s="12">
-        <v>56.46</v>
+        <v>31.6</v>
       </c>
       <c r="F37" s="20">
-        <v>48.92</v>
+        <v>47.33</v>
       </c>
       <c r="G37" s="21">
-        <v>45.92</v>
+        <v>70.97</v>
       </c>
       <c r="H37" s="22">
-        <v>50.45</v>
+        <v>49.97</v>
       </c>
     </row>
     <row r="38" ht="24.7" customHeight="1">
       <c r="A38" s="16">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s" s="17">
         <v>79</v>
@@ -2864,21 +2891,21 @@
         <v>2022</v>
       </c>
       <c r="E38" s="12">
-        <v>31.6</v>
+        <v>46.06</v>
       </c>
       <c r="F38" s="20">
-        <v>47.33</v>
+        <v>48.6</v>
       </c>
       <c r="G38" s="21">
-        <v>70.97</v>
+        <v>45.1</v>
       </c>
       <c r="H38" s="22">
-        <v>49.97</v>
+        <v>46.6</v>
       </c>
     </row>
     <row r="39" ht="24.7" customHeight="1">
       <c r="A39" s="16">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s" s="17">
         <v>81</v>
@@ -2890,21 +2917,21 @@
         <v>2022</v>
       </c>
       <c r="E39" s="12">
-        <v>46.06</v>
+        <v>46.18</v>
       </c>
       <c r="F39" s="20">
-        <v>48.6</v>
+        <v>45.44</v>
       </c>
       <c r="G39" s="21">
-        <v>45.1</v>
+        <v>51.22</v>
       </c>
       <c r="H39" s="22">
-        <v>46.6</v>
+        <v>47.62</v>
       </c>
     </row>
     <row r="40" ht="24.7" customHeight="1">
       <c r="A40" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s" s="17">
         <v>83</v>
@@ -2916,21 +2943,21 @@
         <v>2022</v>
       </c>
       <c r="E40" s="12">
-        <v>46.18</v>
+        <v>44.16</v>
       </c>
       <c r="F40" s="20">
-        <v>45.44</v>
+        <v>52.59</v>
       </c>
       <c r="G40" s="21">
-        <v>51.22</v>
+        <v>47.57</v>
       </c>
       <c r="H40" s="22">
-        <v>47.62</v>
+        <v>48.12</v>
       </c>
     </row>
     <row r="41" ht="24.7" customHeight="1">
       <c r="A41" s="16">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s" s="17">
         <v>85</v>
@@ -2942,21 +2969,21 @@
         <v>2022</v>
       </c>
       <c r="E41" s="12">
-        <v>44.16</v>
+        <v>42.91</v>
       </c>
       <c r="F41" s="20">
-        <v>52.59</v>
+        <v>50.24</v>
       </c>
       <c r="G41" s="21">
-        <v>47.57</v>
+        <v>44.78</v>
       </c>
       <c r="H41" s="22">
-        <v>48.12</v>
+        <v>45.97</v>
       </c>
     </row>
     <row r="42" ht="24.7" customHeight="1">
       <c r="A42" s="16">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s" s="17">
         <v>87</v>
@@ -2968,21 +2995,21 @@
         <v>2022</v>
       </c>
       <c r="E42" s="12">
-        <v>42.91</v>
+        <v>38.13</v>
       </c>
       <c r="F42" s="20">
-        <v>50.24</v>
+        <v>46.2</v>
       </c>
       <c r="G42" s="21">
-        <v>44.78</v>
+        <v>47.76</v>
       </c>
       <c r="H42" s="22">
-        <v>45.97</v>
+        <v>44.02</v>
       </c>
     </row>
     <row r="43" ht="24.7" customHeight="1">
       <c r="A43" s="16">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s" s="17">
         <v>89</v>
@@ -2994,21 +3021,21 @@
         <v>2022</v>
       </c>
       <c r="E43" s="12">
-        <v>38.13</v>
+        <v>63.8</v>
       </c>
       <c r="F43" s="20">
-        <v>46.2</v>
+        <v>47.72</v>
       </c>
       <c r="G43" s="21">
-        <v>47.76</v>
+        <v>45.2</v>
       </c>
       <c r="H43" s="22">
-        <v>44.02</v>
+        <v>52.24</v>
       </c>
     </row>
     <row r="44" ht="24.7" customHeight="1">
       <c r="A44" s="16">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s" s="17">
         <v>91</v>
@@ -3020,21 +3047,21 @@
         <v>2022</v>
       </c>
       <c r="E44" s="12">
-        <v>63.8</v>
+        <v>24.95</v>
       </c>
       <c r="F44" s="20">
-        <v>47.72</v>
+        <v>41.14</v>
       </c>
       <c r="G44" s="21">
-        <v>45.2</v>
+        <v>63.94</v>
       </c>
       <c r="H44" s="22">
-        <v>52.24</v>
+        <v>43.36</v>
       </c>
     </row>
     <row r="45" ht="24.7" customHeight="1">
       <c r="A45" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s" s="17">
         <v>93</v>
@@ -3046,21 +3073,21 @@
         <v>2022</v>
       </c>
       <c r="E45" s="12">
-        <v>24.95</v>
+        <v>58.37</v>
       </c>
       <c r="F45" s="20">
-        <v>41.14</v>
+        <v>46.14</v>
       </c>
       <c r="G45" s="21">
-        <v>63.94</v>
+        <v>45.05</v>
       </c>
       <c r="H45" s="22">
-        <v>43.36</v>
+        <v>49.86</v>
       </c>
     </row>
     <row r="46" ht="24.7" customHeight="1">
       <c r="A46" s="16">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s" s="17">
         <v>95</v>
@@ -3072,21 +3099,21 @@
         <v>2022</v>
       </c>
       <c r="E46" s="12">
-        <v>58.37</v>
+        <v>51.06</v>
       </c>
       <c r="F46" s="20">
-        <v>46.14</v>
+        <v>45.21</v>
       </c>
       <c r="G46" s="21">
-        <v>45.05</v>
+        <v>56.66</v>
       </c>
       <c r="H46" s="22">
-        <v>49.86</v>
+        <v>50.99</v>
       </c>
     </row>
     <row r="47" ht="24.7" customHeight="1">
       <c r="A47" s="16">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s" s="17">
         <v>97</v>
@@ -3098,21 +3125,21 @@
         <v>2022</v>
       </c>
       <c r="E47" s="12">
-        <v>51.06</v>
+        <v>51.93</v>
       </c>
       <c r="F47" s="20">
-        <v>45.21</v>
+        <v>58.99</v>
       </c>
       <c r="G47" s="21">
-        <v>56.66</v>
+        <v>69.84</v>
       </c>
       <c r="H47" s="22">
-        <v>50.99</v>
+        <v>60.24</v>
       </c>
     </row>
     <row r="48" ht="24.7" customHeight="1">
       <c r="A48" s="16">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s" s="17">
         <v>99</v>
@@ -3124,21 +3151,21 @@
         <v>2022</v>
       </c>
       <c r="E48" s="12">
-        <v>51.93</v>
+        <v>45.01</v>
       </c>
       <c r="F48" s="20">
-        <v>58.99</v>
+        <v>52.18</v>
       </c>
       <c r="G48" s="21">
-        <v>69.84</v>
+        <v>47.41</v>
       </c>
       <c r="H48" s="22">
-        <v>60.24</v>
+        <v>48.2</v>
       </c>
     </row>
     <row r="49" ht="24.7" customHeight="1">
       <c r="A49" s="16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s" s="17">
         <v>101</v>
@@ -3150,21 +3177,21 @@
         <v>2022</v>
       </c>
       <c r="E49" s="12">
-        <v>45.01</v>
+        <v>55.14</v>
       </c>
       <c r="F49" s="20">
-        <v>52.18</v>
+        <v>51.98</v>
       </c>
       <c r="G49" s="21">
-        <v>47.41</v>
+        <v>58.4</v>
       </c>
       <c r="H49" s="22">
-        <v>48.2</v>
+        <v>55.16</v>
       </c>
     </row>
     <row r="50" ht="24.7" customHeight="1">
       <c r="A50" s="16">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s" s="17">
         <v>103</v>
@@ -3176,21 +3203,21 @@
         <v>2022</v>
       </c>
       <c r="E50" s="12">
-        <v>55.14</v>
+        <v>53.12</v>
       </c>
       <c r="F50" s="20">
-        <v>51.98</v>
+        <v>56.8</v>
       </c>
       <c r="G50" s="21">
-        <v>58.4</v>
+        <v>55.93</v>
       </c>
       <c r="H50" s="22">
-        <v>55.16</v>
+        <v>55.28</v>
       </c>
     </row>
     <row r="51" ht="24.7" customHeight="1">
       <c r="A51" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s" s="17">
         <v>105</v>
@@ -3202,21 +3229,21 @@
         <v>2022</v>
       </c>
       <c r="E51" s="12">
-        <v>53.12</v>
+        <v>54.02</v>
       </c>
       <c r="F51" s="20">
-        <v>56.8</v>
+        <v>49.06</v>
       </c>
       <c r="G51" s="21">
-        <v>55.93</v>
+        <v>36.04</v>
       </c>
       <c r="H51" s="22">
-        <v>55.28</v>
+        <v>46.37</v>
       </c>
     </row>
     <row r="52" ht="24.7" customHeight="1">
       <c r="A52" s="16">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s" s="17">
         <v>107</v>
@@ -3228,21 +3255,21 @@
         <v>2022</v>
       </c>
       <c r="E52" s="12">
-        <v>54.02</v>
+        <v>48.83</v>
       </c>
       <c r="F52" s="20">
-        <v>49.06</v>
+        <v>52.48</v>
       </c>
       <c r="G52" s="21">
-        <v>36.04</v>
+        <v>56.66</v>
       </c>
       <c r="H52" s="22">
-        <v>46.37</v>
+        <v>52.65</v>
       </c>
     </row>
     <row r="53" ht="24.7" customHeight="1">
       <c r="A53" s="16">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s" s="17">
         <v>109</v>
@@ -3254,41 +3281,15 @@
         <v>2022</v>
       </c>
       <c r="E53" s="12">
-        <v>48.83</v>
+        <v>56.95</v>
       </c>
       <c r="F53" s="20">
-        <v>52.48</v>
+        <v>53.3</v>
       </c>
       <c r="G53" s="21">
-        <v>56.66</v>
+        <v>62.83</v>
       </c>
       <c r="H53" s="22">
-        <v>52.65</v>
-      </c>
-    </row>
-    <row r="54" ht="24.7" customHeight="1">
-      <c r="A54" s="16">
-        <v>56</v>
-      </c>
-      <c r="B54" t="s" s="17">
-        <v>111</v>
-      </c>
-      <c r="C54" t="s" s="18">
-        <v>112</v>
-      </c>
-      <c r="D54" s="19">
-        <v>2022</v>
-      </c>
-      <c r="E54" s="12">
-        <v>56.95</v>
-      </c>
-      <c r="F54" s="20">
-        <v>53.3</v>
-      </c>
-      <c r="G54" s="21">
-        <v>62.83</v>
-      </c>
-      <c r="H54" s="22">
         <v>57.71</v>
       </c>
     </row>
@@ -3296,7 +3297,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E44 E46:E54">
+  <conditionalFormatting sqref="E3:E11">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan" stopIfTrue="1">
       <formula>$R$62</formula>
     </cfRule>
@@ -3308,16 +3309,28 @@
       <formula>$R$64</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E12:E43 E45:E53">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan" stopIfTrue="1">
+      <formula>$R$61</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between" stopIfTrue="1">
+      <formula>$R$61</formula>
+      <formula>$R$62</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan" stopIfTrue="1">
+      <formula>$R$63</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan" stopIfTrue="1">
+      <formula>$Q$61</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between" stopIfTrue="1">
+      <formula>$Q$61</formula>
       <formula>$Q$62</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between" stopIfTrue="1">
-      <formula>$Q$62</formula>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan" stopIfTrue="1">
       <formula>$Q$63</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan" stopIfTrue="1">
-      <formula>$Q$64</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>